<commit_message>
Exclude UID provided widgets from custom widget retrievial on workspace projects
</commit_message>
<xml_diff>
--- a/artifact-counter/summary.xlsx
+++ b/artifact-counter/summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7050" activeTab="1"/>
+    <workbookView windowWidth="24530" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="projects" sheetId="1" r:id="rId1"/>
@@ -226,14 +226,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* \-_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
-    <numFmt numFmtId="178" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* \-??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="0.0_ "/>
+    <numFmt numFmtId="178" formatCode="0.0_ "/>
+    <numFmt numFmtId="179" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,33 +251,18 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -285,13 +270,6 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -310,11 +288,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -342,14 +342,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -357,23 +349,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -387,6 +364,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -394,8 +379,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -416,7 +409,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,7 +505,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,85 +565,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,61 +577,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -610,26 +603,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -649,16 +627,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -681,8 +668,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -697,53 +686,57 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -752,106 +745,106 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -865,10 +858,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="179" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1190,8 +1183,8 @@
   <sheetPr/>
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -1769,7 +1762,7 @@
         <v>3</v>
       </c>
       <c r="K11" s="5">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="L11" s="5">
         <v>3</v>
@@ -1824,7 +1817,7 @@
         <v>2</v>
       </c>
       <c r="K12" s="5">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="L12" s="5">
         <v>0</v>
@@ -1879,7 +1872,7 @@
         <v>1</v>
       </c>
       <c r="K13" s="5">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="L13" s="5">
         <v>0</v>
@@ -1934,7 +1927,7 @@
         <v>23</v>
       </c>
       <c r="K14" s="5">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="L14" s="5">
         <v>14</v>
@@ -1989,7 +1982,7 @@
         <v>14</v>
       </c>
       <c r="K15" s="5">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="L15" s="5">
         <v>67</v>
@@ -2044,7 +2037,7 @@
         <v>1</v>
       </c>
       <c r="K16" s="5">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="L16" s="5">
         <v>0</v>
@@ -2099,7 +2092,7 @@
         <v>73</v>
       </c>
       <c r="K17" s="5">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="L17" s="5">
         <v>1</v>
@@ -2154,7 +2147,7 @@
         <v>36</v>
       </c>
       <c r="K18" s="5">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="L18" s="5">
         <v>2</v>
@@ -2209,7 +2202,7 @@
         <v>2</v>
       </c>
       <c r="K19" s="5">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="L19" s="5">
         <v>0</v>
@@ -2264,7 +2257,7 @@
         <v>2</v>
       </c>
       <c r="K20" s="5">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="L20" s="5">
         <v>0</v>
@@ -2319,7 +2312,7 @@
         <v>1</v>
       </c>
       <c r="K21" s="5">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="L21" s="5">
         <v>0</v>
@@ -2374,7 +2367,7 @@
         <v>76</v>
       </c>
       <c r="K22" s="5">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="L22" s="5">
         <v>39</v>
@@ -2471,8 +2464,8 @@
   <sheetPr/>
   <dimension ref="A1:AC22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A1:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -3376,10 +3369,10 @@
         <v>25</v>
       </c>
       <c r="B11">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="C11">
-        <v>369</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -3465,10 +3458,10 @@
         <v>26</v>
       </c>
       <c r="B12">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -3554,10 +3547,10 @@
         <v>27</v>
       </c>
       <c r="B13">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -3643,10 +3636,10 @@
         <v>28</v>
       </c>
       <c r="B14">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="C14">
-        <v>2047</v>
+        <v>46</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -3732,10 +3725,10 @@
         <v>29</v>
       </c>
       <c r="B15">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="C15">
-        <v>1066</v>
+        <v>110</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -3821,10 +3814,10 @@
         <v>30</v>
       </c>
       <c r="B16">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -3910,10 +3903,10 @@
         <v>31</v>
       </c>
       <c r="B17">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="C17">
-        <v>2056</v>
+        <v>1151</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -3999,10 +3992,10 @@
         <v>32</v>
       </c>
       <c r="B18">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="C18">
-        <v>3396</v>
+        <v>260</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -4088,10 +4081,10 @@
         <v>33</v>
       </c>
       <c r="B19">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -4177,10 +4170,10 @@
         <v>34</v>
       </c>
       <c r="B20">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C20">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -4266,10 +4259,10 @@
         <v>35</v>
       </c>
       <c r="B21">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -4355,10 +4348,10 @@
         <v>36</v>
       </c>
       <c r="B22">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C22">
-        <v>8094</v>
+        <v>333</v>
       </c>
       <c r="D22">
         <v>0</v>

</xml_diff>